<commit_message>
Changed customer under test
</commit_message>
<xml_diff>
--- a/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intellij\18\NetayaSWG\Automation\src\main\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intellij\NewRep\3\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5AC9E8-8333-40C1-BC22-34295013A6F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F3E892-A46F-4B60-9B81-736EFBE972A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="5" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="InstallApplication" sheetId="6" r:id="rId1"/>
@@ -343,10 +343,10 @@
     <t>300</t>
   </si>
   <si>
-    <t>TrustwaveEP Automation #3</t>
-  </si>
-  <si>
     <t>180</t>
+  </si>
+  <si>
+    <t>TrustwaveEP Automation #4</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>62</v>
@@ -1341,13 +1341,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>61</v>
@@ -1364,7 +1364,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1385,7 +1385,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1399,7 +1399,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,7 +1451,7 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Added support for event explorer test of emea/apj + some improvements
</commit_message>
<xml_diff>
--- a/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intellij\NewRep\10\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intellij\NewRep\12\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235C95CF-C903-42D7-B0E5-9A92AFC15DA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21838E1E-A39E-4307-943D-5772CBEC43CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeEPConfigurationTest" sheetId="19" r:id="rId1"/>
-    <sheet name="InstallApplication" sheetId="6" r:id="rId2"/>
-    <sheet name="SAMLTest" sheetId="15" r:id="rId3"/>
-    <sheet name="DownloadFromPortalTest" sheetId="13" r:id="rId4"/>
-    <sheet name="InstallEndPointTest" sheetId="14" r:id="rId5"/>
-    <sheet name="VerifyEndPointOkAtPortalTest" sheetId="16" r:id="rId6"/>
-    <sheet name="ClientLogToPortalTest" sheetId="18" r:id="rId7"/>
-    <sheet name="BlockURLTest" sheetId="8" r:id="rId8"/>
-    <sheet name="BlockEicarTest" sheetId="11" r:id="rId9"/>
-    <sheet name="BlockEicarEnterprise" sheetId="12" r:id="rId10"/>
-    <sheet name="PolicyTest" sheetId="9" r:id="rId11"/>
-    <sheet name="PolicyTestProd" sheetId="10" r:id="rId12"/>
+    <sheet name="DownloadFromPortalTest" sheetId="13" r:id="rId2"/>
+    <sheet name="InstallEndPointTest" sheetId="14" r:id="rId3"/>
+    <sheet name="VerifyEndPointOkAtPortalTest" sheetId="16" r:id="rId4"/>
+    <sheet name="ClientLogToPortalTest" sheetId="21" r:id="rId5"/>
+    <sheet name="General Settings" sheetId="20" r:id="rId6"/>
+    <sheet name="BlockURLTest" sheetId="8" r:id="rId7"/>
+    <sheet name="BlockEicarTest" sheetId="11" r:id="rId8"/>
+    <sheet name="BlockEicarEnterprise" sheetId="12" r:id="rId9"/>
+    <sheet name="PolicyTest" sheetId="9" r:id="rId10"/>
+    <sheet name="PolicyTestProd" sheetId="10" r:id="rId11"/>
+    <sheet name="InstallApplication" sheetId="6" r:id="rId12"/>
+    <sheet name="SAMLTest" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="126">
   <si>
     <t>Description</t>
   </si>
@@ -212,9 +213,6 @@
     <t>Wait files to be downloaded timeout in seconds</t>
   </si>
   <si>
-    <t>120</t>
-  </si>
-  <si>
     <t>Service Start/Stop timeout</t>
   </si>
   <si>
@@ -350,14 +348,86 @@
     <t>TrustwaveEP Automation #3</t>
   </si>
   <si>
-    <t>20</t>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>EMEA</t>
+  </si>
+  <si>
+    <t>APJ</t>
+  </si>
+  <si>
+    <t>AMS</t>
+  </si>
+  <si>
+    <t>Acme San Francisco</t>
+  </si>
+  <si>
+    <t>TWTestEMEA Standalone</t>
+  </si>
+  <si>
+    <t>TWTEST EPAPJ</t>
+  </si>
+  <si>
+    <t>TWTestSupportUser002@trustwave.com</t>
+  </si>
+  <si>
+    <t>we@r3QA!!</t>
+  </si>
+  <si>
+    <t>https://portal.trustwave.com</t>
+  </si>
+  <si>
+    <t>https://fusion.apj.trustwave.com</t>
+  </si>
+  <si>
+    <t>https://portal.emea.trustwave.com</t>
+  </si>
+  <si>
+    <t>https://portal.qa.tw-test.net</t>
+  </si>
+  <si>
+    <t>https://portal.stg.tw-test.net</t>
+  </si>
+  <si>
+    <t>https://portal.inc.tw-test.net</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>INC</t>
+  </si>
+  <si>
+    <t>STG</t>
+  </si>
+  <si>
+    <t>Fusion Link</t>
+  </si>
+  <si>
+    <t>Fusion User Name</t>
+  </si>
+  <si>
+    <t>Fusion Password</t>
+  </si>
+  <si>
+    <t>TWTestEMEA_SupportUser002@trustwave.com</t>
+  </si>
+  <si>
+    <t>uri.hacohen@trustwave.com</t>
+  </si>
+  <si>
+    <t>Ronlove1001</t>
+  </si>
+  <si>
+    <t>TrustwaveEP Test #8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +460,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -412,7 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -422,6 +507,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -737,36 +824,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD07D88-2D09-4EC3-AF84-BB578D4AE2BE}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -776,86 +879,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B53D489-3AD9-4691-BEB7-D49122815826}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="67.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="http://www.eicar.org/download/eicar.com.txt" xr:uid="{0D2BDC67-CF06-40C3-8FC1-AE7EDD91330E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED038C0-817F-472E-AD39-DAEB143C92CB}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -956,7 +979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3590BECC-6F16-49AF-A187-EF8E4637F50A}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1057,7 +1080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC9FAC2-0100-466A-9965-E590FD28E573}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O2"/>
@@ -1182,12 +1205,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370C0B2F-291F-41F7-BBEC-60B7B7B7C290}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,7 +1224,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1210,33 +1233,33 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
-      </c>
-      <c r="H1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>23</v>
@@ -1245,7 +1268,7 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -1253,25 +1276,25 @@
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>25</v>
@@ -1279,25 +1302,25 @@
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>25</v>
@@ -1305,51 +1328,51 @@
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>25</v>
@@ -1368,65 +1391,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC204677-932F-42E3-A329-F307B9A37F9B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" customWidth="1"/>
-    <col min="5" max="5" width="56.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
         <v>54</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1434,7 +1451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28112D5D-4D41-49B5-9C1F-91FA6EFF3BC2}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1451,30 +1468,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1483,33 +1500,295 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2CA0F-1477-46C2-9AA1-8A5670F4E730}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDD2CBB-1A9C-4777-B79F-817AEC5FE145}">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="34.21875" customWidth="1"/>
+    <col min="12" max="12" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{6A2B1639-FFB8-4A56-A462-273BE3BE79F6}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{900CE41B-77AB-4063-8B2B-920DA04888D1}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{F6E0DEF3-3772-418B-B697-BF7BCDF1AC5C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB948423-13E7-4E5E-82C0-F9F18D7DE1F1}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>101</v>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1519,93 +1798,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C3FA84-DBAF-4AD9-B8F6-55B860096D54}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="34.21875" customWidth="1"/>
-    <col min="9" max="9" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21916EB-A6DC-450A-A85F-A34B0CFEF38D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1646,7 +1838,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1658,7 +1850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C4480A-E140-45C4-BF8D-587C885F562F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1738,4 +1930,84 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B53D489-3AD9-4691-BEB7-D49122815826}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="67.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="http://www.eicar.org/download/eicar.com.txt" xr:uid="{0D2BDC67-CF06-40C3-8FC1-AE7EDD91330E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Windows installation working with LNE
</commit_message>
<xml_diff>
--- a/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\2\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\4\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA644EF-1BB6-4C81-BBDC-59B19CDFE0A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4A6D84-F204-45FC-98D0-539AFA41BEF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="SetConfigurationTest" sheetId="22" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="InstallEndPointTest" sheetId="14" r:id="rId4"/>
     <sheet name="VerifyEndPointOkAtPortalTest" sheetId="16" r:id="rId5"/>
     <sheet name="ClientLogToPortalTest" sheetId="21" r:id="rId6"/>
-    <sheet name="General Settings" sheetId="20" r:id="rId7"/>
-    <sheet name="BlockURLTest" sheetId="8" r:id="rId8"/>
-    <sheet name="BlockEicarTest" sheetId="11" r:id="rId9"/>
-    <sheet name="BlockEicarEnterprise" sheetId="12" r:id="rId10"/>
-    <sheet name="PolicyTest" sheetId="9" r:id="rId11"/>
-    <sheet name="PolicyTestProd" sheetId="10" r:id="rId12"/>
-    <sheet name="InstallApplication" sheetId="6" r:id="rId13"/>
-    <sheet name="SAMLTest" sheetId="15" r:id="rId14"/>
+    <sheet name="VerifyInstall" sheetId="23" r:id="rId7"/>
+    <sheet name="General Settings" sheetId="20" r:id="rId8"/>
+    <sheet name="BlockURLTest" sheetId="8" r:id="rId9"/>
+    <sheet name="BlockEicarTest" sheetId="11" r:id="rId10"/>
+    <sheet name="BlockEicarEnterprise" sheetId="12" r:id="rId11"/>
+    <sheet name="PolicyTest" sheetId="9" r:id="rId12"/>
+    <sheet name="PolicyTestProd" sheetId="10" r:id="rId13"/>
+    <sheet name="InstallApplication" sheetId="6" r:id="rId14"/>
+    <sheet name="SAMLTest" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="140">
   <si>
     <t>Description</t>
   </si>
@@ -422,13 +423,123 @@
   </si>
   <si>
     <t>{ "customerId": 1007, "configuration": { "global_conf": { "log_level": "info", "conf_version": 3 }, "agent": { "ds_host": "endpoint-protection-services.local.tw-test.net", "ds_port": 443, "ds_protocol": "https", "check_update_period": 61, "report_period": 60, "ds_max_off_period": 48, "modules": [{ "name": "Windows Log Monitor", "binary_name": "WLM.dll", "enabled": true }, { "name": "Log File Monitor", "binary_name": "LFM.dll", "enabled": true } ], "transport": { "transport_type": 2, "syslog": { "port": 0 }, "scp": { "host": "siem-ingress.trustwave.com", "dest_folder": "/var/siem/data/nep", "port": 9022, "user": "twsiem", "ack": false, "max_send_folder_size": 100 } } }, "wlm": { "max_monitor_queue_size": 10000, "queues_collector_idle_time": 5, "monitor_items": [{ "log_name": "Security", "enabled": true, "advanced_filter": false, "filters": [] }, { "log_name": "System", "enabled": true, "advanced_filter": false, "filters": [] } ] }, "lfm": { "max_monitor_queue_size": 10000, "queues_collector_idle_time": 5, "monitor_items": [] } } }";</t>
+  </si>
+  <si>
+    <t>LNE User Name</t>
+  </si>
+  <si>
+    <t>LNE Password</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>trustwave</t>
+  </si>
+  <si>
+    <t>LNE SSH port</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>LNE File Cabinet Path</t>
+  </si>
+  <si>
+    <t>/work/services/stub-srv/var/file_cabinet/</t>
+  </si>
+  <si>
+    <t>Download folder name</t>
+  </si>
+  <si>
+    <t>C:\SeleniumDownloads</t>
+  </si>
+  <si>
+    <t>EP Installation timeout</t>
+  </si>
+  <si>
+    <t>From EP service start until logs show EP active timeout</t>
+  </si>
+  <si>
+    <t>Download timeout</t>
+  </si>
+  <si>
+    <t>{
+	"customerId": 1001,
+	"configuration": {
+		"centcom_meta": {
+			"schema_version": "1.1.1"
+		},
+		"global_conf": {
+			"log_level": "debug",
+			"conf_version": 3
+		},
+		"agent": {
+			"ds_host": "endpoint-protection-services.local.tw-test.net",
+			"ds_port": 443,
+			"ds_protocol": "https",
+			"check_update_period": 61,
+			"report_period": 60,
+			"ds_max_off_period": 48,
+			"modules": [
+				{
+					"name": "Windows Log Monitor",
+					"binary_name": "WLM.dll",
+					"enabled": true
+				},
+				{
+					"name": "Log File Monitor",
+					"binary_name": "LFM.dll",
+					"enabled": true
+				}
+			],
+			"transport": {
+				"transport_type": 2,
+				"syslog": {
+					"port": 0
+				},
+				"scp": {
+					"host": "siem-ingress.trustwave.com",
+					"dest_folder": "/var/siem/data/nep",
+					"port": 9022,
+					"user": "twsiem",
+					"ack": false,
+					"max_send_folder_size": 100
+				}
+			}
+		},
+		"wlm": {
+			"max_monitor_queue_size": 10000,
+			"queues_collector_idle_time": 5,
+			"monitor_items": [
+				{
+					"log_name": "Security",
+					"enabled": true,
+					"advanced_filter": false,
+					"filters": []
+				},
+				{
+					"log_name": "System",
+					"enabled": true,
+					"advanced_filter": false,
+					"filters": []
+				}
+			]
+		},
+		"lfm": {
+			"max_monitor_queue_size": 10000,
+			"queues_collector_idle_time": 5,
+			"monitor_items": []
+		}
+	}
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,6 +587,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -498,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -510,6 +627,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -827,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F6DEC8-96FE-44EB-BC44-FA92B54DAFB6}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -853,6 +976,88 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C4480A-E140-45C4-BF8D-587C885F562F}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="62.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7DB7016D-EAE0-4F74-9815-03C77405197F}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{2D07E15E-559A-4522-91F2-596B16B3DEF3}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{4CD0DB75-5BED-47C8-AD8D-75AFC5345A0A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B53D489-3AD9-4691-BEB7-D49122815826}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -932,7 +1137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED038C0-817F-472E-AD39-DAEB143C92CB}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1033,7 +1238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3590BECC-6F16-49AF-A187-EF8E4637F50A}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1134,7 +1339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC9FAC2-0100-466A-9965-E590FD28E573}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O2"/>
@@ -1259,7 +1464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370C0B2F-291F-41F7-BBEC-60B7B7B7C290}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -1566,7 +1771,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1644,7 +1849,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1824,11 +2029,46 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB948423-13E7-4E5E-82C0-F9F18D7DE1F1}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35396668-7713-4347-9D9E-B7FEBB13003F}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="70.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB948423-13E7-4E5E-82C0-F9F18D7DE1F1}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1837,9 +2077,16 @@
     <col min="3" max="3" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -1855,8 +2102,29 @@
       <c r="E1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>101</v>
       </c>
@@ -1870,38 +2138,69 @@
         <v>35</v>
       </c>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>116</v>
       </c>
       <c r="E3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>117</v>
       </c>
       <c r="E4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>118</v>
       </c>
       <c r="E5" t="s">
         <v>114</v>
       </c>
+      <c r="H5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21916EB-A6DC-450A-A85F-A34B0CFEF38D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1952,86 +2251,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C4480A-E140-45C4-BF8D-587C885F562F}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="62.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{7DB7016D-EAE0-4F74-9815-03C77405197F}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{2D07E15E-559A-4522-91F2-596B16B3DEF3}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{4CD0DB75-5BED-47C8-AD8D-75AFC5345A0A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added change customer configuration test and merged into SmokeTest.xml suite with install EP test
</commit_message>
<xml_diff>
--- a/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\4\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\5\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4A6D84-F204-45FC-98D0-539AFA41BEF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86891C68-892D-4709-8C33-DFC616D63504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="7" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="SetConfigurationTest" sheetId="22" r:id="rId1"/>
@@ -19,15 +19,16 @@
     <sheet name="InstallEndPointTest" sheetId="14" r:id="rId4"/>
     <sheet name="VerifyEndPointOkAtPortalTest" sheetId="16" r:id="rId5"/>
     <sheet name="ClientLogToPortalTest" sheetId="21" r:id="rId6"/>
-    <sheet name="VerifyInstall" sheetId="23" r:id="rId7"/>
-    <sheet name="General Settings" sheetId="20" r:id="rId8"/>
-    <sheet name="BlockURLTest" sheetId="8" r:id="rId9"/>
-    <sheet name="BlockEicarTest" sheetId="11" r:id="rId10"/>
-    <sheet name="BlockEicarEnterprise" sheetId="12" r:id="rId11"/>
-    <sheet name="PolicyTest" sheetId="9" r:id="rId12"/>
-    <sheet name="PolicyTestProd" sheetId="10" r:id="rId13"/>
-    <sheet name="InstallApplication" sheetId="6" r:id="rId14"/>
-    <sheet name="SAMLTest" sheetId="15" r:id="rId15"/>
+    <sheet name="VerifyWinInstall" sheetId="23" r:id="rId7"/>
+    <sheet name="ChangeCustomerConfiguration" sheetId="24" r:id="rId8"/>
+    <sheet name="General Settings" sheetId="20" r:id="rId9"/>
+    <sheet name="BlockURLTest" sheetId="8" r:id="rId10"/>
+    <sheet name="BlockEicarTest" sheetId="11" r:id="rId11"/>
+    <sheet name="BlockEicarEnterprise" sheetId="12" r:id="rId12"/>
+    <sheet name="PolicyTest" sheetId="9" r:id="rId13"/>
+    <sheet name="PolicyTestProd" sheetId="10" r:id="rId14"/>
+    <sheet name="InstallApplication" sheetId="6" r:id="rId15"/>
+    <sheet name="SAMLTest" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
   <si>
     <t>Description</t>
   </si>
@@ -481,6 +482,79 @@
 			"check_update_period": 61,
 			"report_period": 60,
 			"ds_max_off_period": 48,
+			"modules": [
+				{
+					"name": "Windows Log Monitor",
+					"binary_name": "WLM.dll",
+					"enabled": true
+				},
+				{
+					"name": "Log File Monitor",
+					"binary_name": "LFM.dll",
+					"enabled": true
+				}
+			],
+			"transport": {
+				"transport_type": 2,
+				"syslog": {
+					"port": 0
+				},
+				"scp": {
+					"host": "siem-ingress.trustwave.com",
+					"dest_folder": "/var/siem/data/nep",
+					"port": 9022,
+					"user": "twsiem",
+					"ack": false,
+					"max_send_folder_size": 100
+				}
+			}
+		},
+		"wlm": {
+			"max_monitor_queue_size": 10000,
+			"queues_collector_idle_time": 5,
+			"monitor_items": [
+				{
+					"log_name": "Security",
+					"enabled": true,
+					"advanced_filter": false,
+					"filters": []
+				},
+				{
+					"log_name": "System",
+					"enabled": true,
+					"advanced_filter": false,
+					"filters": []
+				}
+			]
+		},
+		"lfm": {
+			"max_monitor_queue_size": 10000,
+			"queues_collector_idle_time": 5,
+			"monitor_items": []
+		}
+	}
+}</t>
+  </si>
+  <si>
+    <t>EP Service Timeout</t>
+  </si>
+  <si>
+    <t>{
+	"customerId": 1001,
+	"configuration": {
+		"centcom_meta": {
+			"schema_version": "1.1.1"
+		},
+		"global_conf": {
+			"log_level": "debug"
+		},
+		"agent": {
+			"ds_host": "endpoint-protection-services.local.tw-test.net",
+			"ds_port": 443,
+			"ds_protocol": "https",
+			"check_update_period": 31,
+			"report_period": 35,
+			"ds_max_off_period": 24,
 			"modules": [
 				{
 					"name": "Windows Log Monitor",
@@ -976,6 +1050,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21916EB-A6DC-450A-A85F-A34B0CFEF38D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="http://example.com" xr:uid="{025340AC-6526-4720-9476-EB638351E888}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C4480A-E140-45C4-BF8D-587C885F562F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1057,7 +1184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B53D489-3AD9-4691-BEB7-D49122815826}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1137,7 +1264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED038C0-817F-472E-AD39-DAEB143C92CB}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1238,7 +1365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3590BECC-6F16-49AF-A187-EF8E4637F50A}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1339,7 +1466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC9FAC2-0100-466A-9965-E590FD28E573}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O2"/>
@@ -1464,7 +1591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370C0B2F-291F-41F7-BBEC-60B7B7B7C290}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -2033,7 +2160,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2054,7 +2181,7 @@
         <v>139</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2064,11 +2191,46 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1226C161-6D55-4F3D-A153-054D109DEBD4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="70.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB948423-13E7-4E5E-82C0-F9F18D7DE1F1}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,7 +2248,7 @@
     <col min="12" max="12" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2123,8 +2285,11 @@
       <c r="L1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>101</v>
       </c>
@@ -2159,8 +2324,11 @@
       <c r="L2" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>116</v>
       </c>
@@ -2171,7 +2339,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>117</v>
       </c>
@@ -2182,7 +2350,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>118</v>
       </c>
@@ -2198,57 +2366,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21916EB-A6DC-450A-A85F-A34B0CFEF38D}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="http://example.com" xr:uid="{025340AC-6526-4720-9476-EB638351E888}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed issues withsmoke suite was not checking the right test
</commit_message>
<xml_diff>
--- a/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\5\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\11\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86891C68-892D-4709-8C33-DFC616D63504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BE43B1-380A-4B89-AD2F-AB1BCD87906D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="7" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
@@ -552,8 +552,8 @@
 			"ds_host": "endpoint-protection-services.local.tw-test.net",
 			"ds_port": 443,
 			"ds_protocol": "https",
-			"check_update_period": 31,
-			"report_period": 35,
+			"check_update_period": 33,
+			"report_period": 31,
 			"ds_max_off_period": 24,
 			"modules": [
 				{
@@ -2194,7 +2194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1226C161-6D55-4F3D-A153-054D109DEBD4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added loop waiting for LNE to load for the first time
</commit_message>
<xml_diff>
--- a/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\11\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\13\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BE43B1-380A-4B89-AD2F-AB1BCD87906D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197C749E-9C75-43E0-A904-FAA4182AAC75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="7" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="6" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="SetConfigurationTest" sheetId="22" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="143">
   <si>
     <t>Description</t>
   </si>
@@ -552,8 +552,8 @@
 			"ds_host": "endpoint-protection-services.local.tw-test.net",
 			"ds_port": 443,
 			"ds_protocol": "https",
-			"check_update_period": 33,
-			"report_period": 31,
+			"check_update_period": 31,
+			"report_period": 32,
 			"ds_max_off_period": 24,
 			"modules": [
 				{
@@ -607,6 +607,9 @@
 		}
 	}
 }</t>
+  </si>
+  <si>
+    <t>From LNE up until response OK timeout</t>
   </si>
 </sst>
 </file>
@@ -2157,31 +2160,38 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35396668-7713-4347-9D9E-B7FEBB13003F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="70.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>124</v>
       </c>
       <c r="B1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>99</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2194,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1226C161-6D55-4F3D-A153-054D109DEBD4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
LNE smoke improvements and bug fixes
</commit_message>
<xml_diff>
--- a/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\13\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\16\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197C749E-9C75-43E0-A904-FAA4182AAC75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242A9E0F-684E-4F3B-AFC1-EA1B6301DACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="6" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="5" activeTab="8" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="SetConfigurationTest" sheetId="22" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="141">
   <si>
     <t>Description</t>
   </si>
@@ -442,12 +442,6 @@
   </si>
   <si>
     <t>22</t>
-  </si>
-  <si>
-    <t>LNE File Cabinet Path</t>
-  </si>
-  <si>
-    <t>/work/services/stub-srv/var/file_cabinet/</t>
   </si>
   <si>
     <t>Download folder name</t>
@@ -2162,7 +2156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35396668-7713-4347-9D9E-B7FEBB13003F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2177,15 +2171,15 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>99</v>
@@ -2218,12 +2212,12 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>99</v>
@@ -2237,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB948423-13E7-4E5E-82C0-F9F18D7DE1F1}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2252,13 +2246,12 @@
     <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2290,16 +2283,13 @@
         <v>134</v>
       </c>
       <c r="K1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>101</v>
       </c>
@@ -2325,8 +2315,8 @@
       <c r="I2" t="s">
         <v>133</v>
       </c>
-      <c r="J2" t="s">
-        <v>135</v>
+      <c r="J2" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>99</v>
@@ -2334,11 +2324,8 @@
       <c r="L2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>116</v>
       </c>
@@ -2346,10 +2333,10 @@
         <v>113</v>
       </c>
       <c r="H3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>117</v>
       </c>
@@ -2357,10 +2344,10 @@
         <v>115</v>
       </c>
       <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>118</v>
       </c>
@@ -2368,8 +2355,8 @@
         <v>114</v>
       </c>
       <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Changed configuration json for next
</commit_message>
<xml_diff>
--- a/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
+++ b/nep-qa-automation/src/main/java/DataFiles/DataFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\16\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extentions\fixNext\nep-qa\nep-qa-automation\src\main\java\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242A9E0F-684E-4F3B-AFC1-EA1B6301DACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C407A687-4201-4F58-B0B6-E9ABDCE2FA13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="5" activeTab="8" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="5" activeTab="6" xr2:uid="{0813270D-BFFB-4065-B4A0-DD50BA55F9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="SetConfigurationTest" sheetId="22" r:id="rId1"/>
@@ -459,6 +459,12 @@
     <t>Download timeout</t>
   </si>
   <si>
+    <t>EP Service Timeout</t>
+  </si>
+  <si>
+    <t>From LNE up until response OK timeout</t>
+  </si>
+  <si>
     <t>{
 	"customerId": 1001,
 	"configuration": {
@@ -466,16 +472,15 @@
 			"schema_version": "1.1.1"
 		},
 		"global_conf": {
-			"log_level": "debug",
-			"conf_version": 3
+			"log_level": "debug"
 		},
 		"agent": {
 			"ds_host": "endpoint-protection-services.local.tw-test.net",
 			"ds_port": 443,
 			"ds_protocol": "https",
-			"check_update_period": 61,
-			"report_period": 60,
-			"ds_max_off_period": 48,
+			"check_update_period": 31,
+			"report_period": 32,
+			"ds_max_off_period": 24,
 			"modules": [
 				{
 					"name": "Windows Log Monitor",
@@ -489,7 +494,7 @@
 				}
 			],
 			"transport": {
-				"transport_type": 2,
+				"server_type": 1,
 				"syslog": {
 					"port": 0
 				},
@@ -530,9 +535,6 @@
 }</t>
   </si>
   <si>
-    <t>EP Service Timeout</t>
-  </si>
-  <si>
     <t>{
 	"customerId": 1001,
 	"configuration": {
@@ -540,15 +542,16 @@
 			"schema_version": "1.1.1"
 		},
 		"global_conf": {
-			"log_level": "debug"
+			"log_level": "debug",
+			"conf_version": 3
 		},
 		"agent": {
 			"ds_host": "endpoint-protection-services.local.tw-test.net",
 			"ds_port": 443,
 			"ds_protocol": "https",
-			"check_update_period": 31,
-			"report_period": 32,
-			"ds_max_off_period": 24,
+			"check_update_period": 61,
+			"report_period": 60,
+			"ds_max_off_period": 48,
 			"modules": [
 				{
 					"name": "Windows Log Monitor",
@@ -562,7 +565,7 @@
 				}
 			],
 			"transport": {
-				"transport_type": 2,
+				"server_type": 1,
 				"syslog": {
 					"port": 0
 				},
@@ -601,9 +604,6 @@
 		}
 	}
 }</t>
-  </si>
-  <si>
-    <t>From LNE up until response OK timeout</t>
   </si>
 </sst>
 </file>
@@ -2156,8 +2156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35396668-7713-4347-9D9E-B7FEBB13003F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2174,12 +2174,12 @@
         <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>99</v>
@@ -2233,8 +2233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB948423-13E7-4E5E-82C0-F9F18D7DE1F1}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2286,7 +2286,7 @@
         <v>135</v>
       </c>
       <c r="L1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>